<commit_message>
#1 Added test case to test displaying of main menu
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\ETI Assignment\ETIAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D364D82-C7B6-40AD-9884-8FDE04D9814E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D7AE98-6D6C-47B2-A485-FDA5F185051D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="9600" windowHeight="4920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="73">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Program will continue to start the correct action after option is entered.</t>
   </si>
   <si>
-    <t>Test invalid option entered triggers validation.</t>
-  </si>
-  <si>
     <t>Program will display validation that invalid option has been entered and prompts user to try again.</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t xml:space="preserve">To test if endpoint can be created successfully. </t>
   </si>
   <si>
-    <t>Test valid option entered triggers correct ouput</t>
-  </si>
-  <si>
     <t>Program will print amount of lines that is present in the excel file.</t>
   </si>
   <si>
@@ -100,12 +94,6 @@
   </si>
   <si>
     <t>Test returning to main menu while playing the maze</t>
-  </si>
-  <si>
-    <t>To test if the program detects the right options when valid options are keyed in.</t>
-  </si>
-  <si>
-    <t>To test if the program is able to detect that invalid option is entered and is able to show validations.</t>
   </si>
   <si>
     <t>To test if the program is able to load and read the correct number of lines that is present in the excel file.</t>
@@ -274,6 +262,27 @@
   </si>
   <si>
     <t>Program will show the Configure Menu.</t>
+  </si>
+  <si>
+    <t>Test valid main menu option entered triggers correct ouput</t>
+  </si>
+  <si>
+    <t>To test if the program detects the right options for the main menu when valid options are keyed in.</t>
+  </si>
+  <si>
+    <t>Test invalid main menu option entered triggers validation.</t>
+  </si>
+  <si>
+    <t>To test if the program is able to detect that invalid option for the main menu is entered and is able to show validations.</t>
+  </si>
+  <si>
+    <t>Test displaying of main menu</t>
+  </si>
+  <si>
+    <t>To test if the program is able to display the main menu successfully.</t>
+  </si>
+  <si>
+    <t>Program will display the main menu</t>
   </si>
 </sst>
 </file>
@@ -652,23 +661,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="58.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="17.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="4.41015625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="44.87890625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.1171875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="58.703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.703125" style="2" customWidth="1"/>
+    <col min="6" max="7" width="17.41015625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.5859375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.1171875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -694,21 +703,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>6</v>
@@ -720,21 +729,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="43" x14ac:dyDescent="0.5">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>6</v>
@@ -746,21 +755,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>6</v>
@@ -772,7 +781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="43" x14ac:dyDescent="0.5">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -780,13 +789,13 @@
         <v>17</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>6</v>
@@ -798,21 +807,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="43" x14ac:dyDescent="0.5">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>6</v>
@@ -824,21 +833,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="43" x14ac:dyDescent="0.5">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>6</v>
@@ -850,7 +859,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="43" x14ac:dyDescent="0.5">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -858,13 +867,13 @@
         <v>20</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>6</v>
@@ -876,21 +885,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>42</v>
+        <v>24</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>6</v>
@@ -902,21 +911,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>6</v>
@@ -928,22 +937,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="F11" s="4" t="s">
         <v>6</v>
       </c>
@@ -954,21 +963,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>6</v>
@@ -980,21 +989,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>6</v>
@@ -1006,21 +1015,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>6</v>
@@ -1032,21 +1041,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>6</v>
@@ -1058,21 +1067,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>6</v>
@@ -1084,10 +1093,36 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A21" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#1 made minor changes
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\ETI Assignment\ETIAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D7AE98-6D6C-47B2-A485-FDA5F185051D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188E58AB-ECF2-4CDA-A426-FC8E40BE0477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -146,14 +146,6 @@
   </si>
   <si>
     <t>Input: 
-Option - 1/2/3/4/0</t>
-  </si>
-  <si>
-    <t>Input: 
-Option - 5/6/7/8/9</t>
-  </si>
-  <si>
-    <t>Input: 
 Option - 3
 Movement Key - F</t>
   </si>
@@ -264,18 +256,9 @@
     <t>Program will show the Configure Menu.</t>
   </si>
   <si>
-    <t>Test valid main menu option entered triggers correct ouput</t>
-  </si>
-  <si>
-    <t>To test if the program detects the right options for the main menu when valid options are keyed in.</t>
-  </si>
-  <si>
     <t>Test invalid main menu option entered triggers validation.</t>
   </si>
   <si>
-    <t>To test if the program is able to detect that invalid option for the main menu is entered and is able to show validations.</t>
-  </si>
-  <si>
     <t>Test displaying of main menu</t>
   </si>
   <si>
@@ -283,6 +266,23 @@
   </si>
   <si>
     <t>Program will display the main menu</t>
+  </si>
+  <si>
+    <t>To test if the program accepts a valid input for main menu selection.</t>
+  </si>
+  <si>
+    <t>To test if the program triggers validation for an invalid input for main menu selection.</t>
+  </si>
+  <si>
+    <t>Input: 
+Option - 0</t>
+  </si>
+  <si>
+    <t>Test valid main menu option is accepted</t>
+  </si>
+  <si>
+    <t>Input: 
+Option - 5</t>
   </si>
 </sst>
 </file>
@@ -661,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -708,16 +708,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>6</v>
@@ -734,13 +734,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>10</v>
@@ -760,13 +760,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>11</v>
@@ -896,7 +896,7 @@
         <v>24</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>28</v>
@@ -922,10 +922,10 @@
         <v>30</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>6</v>
@@ -942,16 +942,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>6</v>
@@ -968,16 +968,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="E12" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>6</v>
@@ -994,16 +994,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="E13" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>6</v>
@@ -1020,16 +1020,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="E14" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>6</v>
@@ -1046,16 +1046,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>6</v>
@@ -1072,16 +1072,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>6</v>
@@ -1098,16 +1098,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
#3 Updated test_outputs.jpg and TestCases.xlsx
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\ETI Assignment\ETIAssignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\ETIAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188E58AB-ECF2-4CDA-A426-FC8E40BE0477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378A0CE9-452D-4C84-A343-F79DE63B97AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="75">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -283,6 +283,12 @@
   <si>
     <t>Input: 
 Option - 5</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Same as expected outcome.</t>
   </si>
 </sst>
 </file>
@@ -661,23 +667,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.41015625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="44.87890625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.1171875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="58.703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.703125" style="2" customWidth="1"/>
-    <col min="6" max="7" width="17.41015625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="24.5859375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.1171875" style="2"/>
+    <col min="1" max="1" width="4.36328125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="44.90625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.08984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="58.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.7265625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="17.36328125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.54296875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.08984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -703,7 +709,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -720,16 +726,16 @@
         <v>67</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -746,16 +752,16 @@
         <v>10</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -772,16 +778,16 @@
         <v>11</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -807,7 +813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="43" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -833,7 +839,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="43" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -859,7 +865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -885,7 +891,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -911,7 +917,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -937,7 +943,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -963,7 +969,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -989,7 +995,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1015,7 +1021,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1041,7 +1047,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1067,7 +1073,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1093,7 +1099,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1119,10 +1125,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:8" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#4 Updated test_outputs.jpg and TestCase.xlsx
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\ETIAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378A0CE9-452D-4C84-A343-F79DE63B97AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39513ED3-9B7F-4EC9-A675-38513EF315C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -668,7 +668,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F4"/>
+      <selection activeCell="G4" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -804,10 +804,10 @@
         <v>14</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
#5 Updated test_outputs.jpg and TestCases.xlsx
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\ETIAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39513ED3-9B7F-4EC9-A675-38513EF315C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE7F197-1569-4A0C-97D9-D79687B3A269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -668,7 +668,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G5"/>
+      <selection activeCell="G5" sqref="G5:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -830,10 +830,10 @@
         <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
#2 Committed test scripts and test outputs for 6.0 and 8.0, updated justification for 7.0
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\ETIAssignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\ETI Assignment\test2\ETIAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE7F197-1569-4A0C-97D9-D79687B3A269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3AFBA9-7D51-4253-B9B2-B94A0EB125B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5010" yWindow="4170" windowWidth="21600" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="76">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Same as expected outcome.</t>
+  </si>
+  <si>
+    <t>Cannot be done as the program cannot read the console while asking for an input.</t>
   </si>
 </sst>
 </file>
@@ -400,6 +403,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>145676</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>347381</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4751294</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>3109808</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BADBABA-7F63-4FFF-8A5E-7406A0686CAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13794441" y="4347881"/>
+          <a:ext cx="4605618" cy="2762427"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -667,23 +719,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G6"/>
+    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="44.90625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.08984375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="58.7265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.7265625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="17.36328125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="24.54296875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.08984375" style="2"/>
+    <col min="1" max="1" width="4.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="58.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="17.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="78.42578125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -709,7 +761,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -735,7 +787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -761,7 +813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -787,7 +839,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -813,7 +865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -839,7 +891,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -865,7 +917,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="254.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -885,13 +937,13 @@
         <v>6</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -917,7 +969,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -943,7 +995,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -969,7 +1021,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -995,7 +1047,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1021,7 +1073,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1047,7 +1099,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1073,7 +1125,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1099,7 +1151,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1125,14 +1177,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#2 Commited test scripts, test outputs and test case for 7.0
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\ETI Assignment\test2\ETIAssignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\ETI Assignment\test3\ETIAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3AFBA9-7D51-4253-B9B2-B94A0EB125B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47E4448-58C2-4EF2-AD62-6A283F443948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5010" yWindow="4170" windowWidth="21600" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="75">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -289,9 +289,6 @@
   </si>
   <si>
     <t>Same as expected outcome.</t>
-  </si>
-  <si>
-    <t>Cannot be done as the program cannot read the console while asking for an input.</t>
   </si>
 </sst>
 </file>
@@ -403,55 +400,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>145676</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>347381</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>4751294</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>3109808</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BADBABA-7F63-4FFF-8A5E-7406A0686CAF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13794441" y="4347881"/>
-          <a:ext cx="4605618" cy="2762427"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -719,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,7 +865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="254.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -937,10 +885,10 @@
         <v>6</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1186,6 +1134,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#6 updated test_outputs.jpg and TestCases.xlsx
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\ETI Assignment\test3\ETIAssignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\ETIAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47E4448-58C2-4EF2-AD62-6A283F443948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5110695-A97C-47A8-B48C-C6B08BB149BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -400,6 +400,54 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>37355</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>50651</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3955853</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2054410</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{961E607C-EF6F-4D5C-8320-BE87C3FBE3ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect r="25354"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11967884" y="3741122"/>
+          <a:ext cx="3918498" cy="2003759"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -667,23 +715,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="58.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="17.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="78.42578125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="4.453125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="44.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="58.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.54296875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="57" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="78.453125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -709,7 +758,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -735,7 +784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -761,7 +810,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -787,7 +836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -813,7 +862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -839,7 +888,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -856,16 +905,16 @@
         <v>26</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="165.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -881,9 +930,7 @@
       <c r="E8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
         <v>9</v>
       </c>
@@ -891,7 +938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -908,16 +955,16 @@
         <v>28</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -943,7 +990,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -969,7 +1016,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -995,7 +1042,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1021,7 +1068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1047,7 +1094,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1073,7 +1120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1099,7 +1146,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1125,14 +1172,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#6 #2 updated TestCases.xlsx and test_maze.py
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\ETIAssignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\ETI Assignment\test3\ETIAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5110695-A97C-47A8-B48C-C6B08BB149BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7CEAA4-86B1-44A2-909C-4D58FDACA523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="76">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Same as expected outcome.</t>
+  </si>
+  <si>
+    <t>Will not be doable as console output cannot be captured while the program is asking for an input.</t>
   </si>
 </sst>
 </file>
@@ -400,54 +403,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>37355</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>50651</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>3955853</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>2054410</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{961E607C-EF6F-4D5C-8320-BE87C3FBE3ED}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect r="25354"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11967884" y="3741122"/>
-          <a:ext cx="3918498" cy="2003759"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -716,23 +671,23 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.453125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="44.81640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.1796875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="58.7265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.54296875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="57" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="78.453125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="4.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="58.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="78.42578125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -758,7 +713,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -784,7 +739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -810,7 +765,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -836,7 +791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -862,7 +817,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -888,7 +843,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -914,7 +869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="165.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -930,15 +885,17 @@
       <c r="E8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="G8" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -964,7 +921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -990,7 +947,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1016,7 +973,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1042,7 +999,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1068,7 +1025,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1094,7 +1051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1120,7 +1077,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1146,7 +1103,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1172,15 +1129,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#2 Commited test scripts, test outputs and test case for configure maze
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\ETI Assignment\test3\ETIAssignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geral\Desktop\ETIAssignment\ETIAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7CEAA4-86B1-44A2-909C-4D58FDACA523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FD3012-5180-4F4D-9583-34AB1FC85688}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="0" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -154,57 +154,15 @@
 Option - 4</t>
   </si>
   <si>
-    <t>Test exiting current configuration and back into Configure Menu.</t>
-  </si>
-  <si>
-    <t>Input:
-Option - 4
-Configure Menu Option - 1/2/3/4
-'B'</t>
-  </si>
-  <si>
-    <t>Test exiting current configuration and back in to Main Menu</t>
-  </si>
-  <si>
-    <t>To test if the program is able to correct return to the Main Menu from the current configuration.</t>
-  </si>
-  <si>
-    <t>To test if the program is able to correctly return to Configure Menu from the current configuration.</t>
-  </si>
-  <si>
-    <t>Input:
-Option - 4
-Configure Menu Option - 1/2/3/4
-'M'</t>
-  </si>
-  <si>
-    <t>Program will return to the Main Menu.</t>
-  </si>
-  <si>
-    <t>Program will return to Configure Menu.</t>
-  </si>
-  <si>
     <t>Test creation of walls</t>
   </si>
   <si>
     <t>To test if walls can be created successfully.</t>
   </si>
   <si>
-    <t>Input:
-Option - 4
-Configure Menu Option - 1
-Coordinates - 1,1</t>
-  </si>
-  <si>
     <t>There should be an 'O' at the coordinates specified.</t>
   </si>
   <si>
-    <t>To test if validation is present when an invalid coordinate is entered</t>
-  </si>
-  <si>
-    <t>Program will display an error message which says that the coordinates entered is invalid.</t>
-  </si>
-  <si>
     <t>Test creation of passageways</t>
   </si>
   <si>
@@ -214,19 +172,7 @@
     <t>There should be an 'X' at the coordinates specified.</t>
   </si>
   <si>
-    <t>Input:
-Option - 4
-Configure Menu Option - 2
-Coordinates - 2,2</t>
-  </si>
-  <si>
     <t>There should be an 'A' at the coordinates specified and the previous start point (if any) will be updated to an 'O'.</t>
-  </si>
-  <si>
-    <t>Input:
-Option - 4
-Configure Menu Option - 3
-Coordinates - 1,7</t>
   </si>
   <si>
     <t>Test creation of start point</t>
@@ -244,54 +190,63 @@
     <t>There should be an 'B' at the coordinates specified and the previous end point (if any) will be updated to an 'O'.</t>
   </si>
   <si>
-    <t>Test invalid input when configuring the maze</t>
+    <t>Program will show the Configure Menu.</t>
+  </si>
+  <si>
+    <t>Test invalid main menu option entered triggers validation.</t>
+  </si>
+  <si>
+    <t>Test displaying of main menu</t>
+  </si>
+  <si>
+    <t>To test if the program is able to display the main menu successfully.</t>
+  </si>
+  <si>
+    <t>Program will display the main menu</t>
+  </si>
+  <si>
+    <t>To test if the program accepts a valid input for main menu selection.</t>
+  </si>
+  <si>
+    <t>To test if the program triggers validation for an invalid input for main menu selection.</t>
+  </si>
+  <si>
+    <t>Input: 
+Option - 0</t>
+  </si>
+  <si>
+    <t>Test valid main menu option is accepted</t>
+  </si>
+  <si>
+    <t>Input: 
+Option - 5</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Same as expected outcome.</t>
+  </si>
+  <si>
+    <t>Will not be doable as console output cannot be captured while the program is asking for an input.</t>
   </si>
   <si>
     <t>Input:
 Option - 4
-Configure Menu Option - 1/2/3/4
-Coordinates - 9,1</t>
-  </si>
-  <si>
-    <t>Program will show the Configure Menu.</t>
-  </si>
-  <si>
-    <t>Test invalid main menu option entered triggers validation.</t>
-  </si>
-  <si>
-    <t>Test displaying of main menu</t>
-  </si>
-  <si>
-    <t>To test if the program is able to display the main menu successfully.</t>
-  </si>
-  <si>
-    <t>Program will display the main menu</t>
-  </si>
-  <si>
-    <t>To test if the program accepts a valid input for main menu selection.</t>
-  </si>
-  <si>
-    <t>To test if the program triggers validation for an invalid input for main menu selection.</t>
-  </si>
-  <si>
-    <t>Input: 
-Option - 0</t>
-  </si>
-  <si>
-    <t>Test valid main menu option is accepted</t>
-  </si>
-  <si>
-    <t>Input: 
-Option - 5</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Same as expected outcome.</t>
-  </si>
-  <si>
-    <t>Will not be doable as console output cannot be captured while the program is asking for an input.</t>
+Configure Menu Option - 1
+Coordinates - 2,2</t>
+  </si>
+  <si>
+    <t>Input:
+Option - 4
+Configure Menu Option - 2
+Coordinates - 3,2</t>
+  </si>
+  <si>
+    <t>Input:
+Option - 4
+Configure Menu Option - 3
+Coordinates - 1,1</t>
   </si>
 </sst>
 </file>
@@ -668,26 +623,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="58.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="78.42578125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="4.453125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="44.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="58.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.54296875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="34.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="78.453125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -713,85 +668,85 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -808,16 +763,16 @@
         <v>14</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -834,16 +789,16 @@
         <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -860,16 +815,16 @@
         <v>26</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -892,10 +847,10 @@
         <v>6</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -912,16 +867,16 @@
         <v>28</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -935,7 +890,7 @@
         <v>36</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>6</v>
@@ -947,7 +902,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -955,13 +910,13 @@
         <v>37</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>6</v>
@@ -973,21 +928,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>6</v>
@@ -999,21 +954,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>6</v>
@@ -1025,21 +980,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>6</v>
@@ -1051,89 +1006,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+    <row r="16" spans="1:8" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
+    </row>
+    <row r="17" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#7 updated test outputs and test cases
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geral\Desktop\ETIAssignment\ETIAssignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\ETIAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FD3012-5180-4F4D-9583-34AB1FC85688}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8C5280-DB06-45C9-B665-92816149167A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="0" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -247,6 +247,9 @@
 Option - 4
 Configure Menu Option - 3
 Coordinates - 1,1</t>
+  </si>
+  <si>
+    <t>OSError: reading from stdin while output is captured</t>
   </si>
 </sst>
 </file>
@@ -625,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -893,7 +896,7 @@
         <v>48</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>9</v>
@@ -919,10 +922,10 @@
         <v>42</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>6</v>
@@ -945,10 +948,10 @@
         <v>39</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>6</v>
@@ -971,10 +974,10 @@
         <v>43</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>6</v>
@@ -997,10 +1000,10 @@
         <v>47</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
#7 #2 updated test script and test cases
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\ETIAssignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geral\Desktop\test\ETIASSignment\ETIAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8C5280-DB06-45C9-B665-92816149167A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B6D653-6C5A-42EA-8FFD-8AE4500E287C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Justifications (if any)</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>Program will continue to start the correct action after option is entered.</t>
@@ -228,9 +225,6 @@
     <t>Same as expected outcome.</t>
   </si>
   <si>
-    <t>Will not be doable as console output cannot be captured while the program is asking for an input.</t>
-  </si>
-  <si>
     <t>Input:
 Option - 4
 Configure Menu Option - 1
@@ -249,7 +243,8 @@
 Coordinates - 1,1</t>
   </si>
   <si>
-    <t>OSError: reading from stdin while output is captured</t>
+    <t>Will not be doable as console output cannot be captured while the program is asking for an input. It will trigger the following error:
+- OSError: reading from stdin while output is captured</t>
   </si>
 </sst>
 </file>
@@ -628,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:G14"/>
+    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -676,22 +671,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>6</v>
@@ -702,22 +697,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>6</v>
@@ -728,22 +723,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>6</v>
@@ -754,22 +749,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>6</v>
@@ -780,22 +775,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>6</v>
@@ -806,22 +801,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>6</v>
@@ -832,16 +827,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>6</v>
@@ -850,7 +845,7 @@
         <v>6</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
@@ -858,51 +853,51 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
@@ -910,22 +905,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="D11" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>6</v>
@@ -936,22 +931,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>6</v>
@@ -962,22 +957,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>6</v>
@@ -988,22 +983,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="F14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>6</v>

</xml_diff>